<commit_message>
Code cleanup and test plan updated
</commit_message>
<xml_diff>
--- a/research/abstractionAnalysis/testfiles/Test Cases Documentation.xlsx
+++ b/research/abstractionAnalysis/testfiles/Test Cases Documentation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jisoo\Documents\GitHub\POET-git\research\abstractionAnalysis\testfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2742B4A8-B7E2-46EF-BAD9-EFE0D6C31BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44BAEDDA-8141-4495-8DA4-7B041C74905E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E5BCCA45-9092-4AE7-83FF-668904ED864A}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
   <si>
     <t>Test No.</t>
   </si>
@@ -43,23 +43,179 @@
     <t>Test Scenario</t>
   </si>
   <si>
-    <t>Test Steps</t>
-  </si>
-  <si>
     <t>Pre-Condition</t>
   </si>
   <si>
-    <t>Expected Results</t>
-  </si>
-  <si>
     <t>Post-Condition</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>Expected Output</t>
+  </si>
+  <si>
+    <t>Actual Output</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>PositionVariablesOfAbstraction(data_a) returns position variables</t>
+  </si>
+  <si>
+    <t>data_a = front ZeroOrMoreData back NULL</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>For all variables v in each internal state of the abstraction, if v is not followed by ..., then v is a position variable.</t>
+  </si>
+  <si>
+    <t>ZeroOrMoreData = elem …</t>
+  </si>
+  <si>
+    <t>data_a = top ZeroOrMoreData NULL</t>
+  </si>
+  <si>
+    <t>data_a = NULL</t>
+  </si>
+  <si>
+    <t>p_v = NULL</t>
+  </si>
+  <si>
+    <t>data_a = ZeroOrMoreData</t>
+  </si>
+  <si>
+    <t>PointerMemberVariablesOfClass(vars_i) returns pointer variables of class</t>
+  </si>
+  <si>
+    <t>vars_i = TypeInfo#(
+  PtrType#TypeName#(
+      "SinglyLinkedEntryWrap",
+      TemplateInstantiation#"T"),
+  "next",
+  "")
+TypeInfo#(
+  "T",
+  "o",
+  "")
+ NULL</t>
+  </si>
+  <si>
+    <t>vars_i = TypeInfo#(
+  IntType1#"unsigned",
+  "count",
+  "")
+TypeInfo#(
+  PtrType#TypeName#(
+      "SinglyLinkedEntryWrap",
+      TemplateInstantiation#"T"),
+  "head",
+  "")
+TypeInfo#(
+  PtrType#TypeName#(
+      "SinglyLinkedEntryWrap",
+      TemplateInstantiation#"T"),
+  "end",
+  "")
+ NULL</t>
+  </si>
+  <si>
+    <t>vars_i = NULL</t>
+  </si>
+  <si>
+    <t>p_i = NULL</t>
+  </si>
+  <si>
+    <t>PossibleMappings(p_v, p_i) returns pairs of one p_v and one p_i</t>
+  </si>
+  <si>
+    <t>p_v = "front" "back"</t>
+  </si>
+  <si>
+    <t>p_v = "top"</t>
+  </si>
+  <si>
+    <t>p_i = "next"</t>
+  </si>
+  <si>
+    <t>p_i = "end" "head"</t>
+  </si>
+  <si>
+    <t>C++ class: SinglyLinkedList</t>
+  </si>
+  <si>
+    <t>Abstraction: Queue, Stack</t>
+  </si>
+  <si>
+    <t>p_v = "front" "back"
+p_i = "end" "head"</t>
+  </si>
+  <si>
+    <t>p_v = "top"
+p_i = "end" "head"</t>
+  </si>
+  <si>
+    <t>p_v = "front" "back"
+p_i = "next"</t>
+  </si>
+  <si>
+    <t>p_v = "top"
+p_i = "next"</t>
+  </si>
+  <si>
+    <t>f_v = "front" "end", "front" "head", "back" "end", "back" "head"</t>
+  </si>
+  <si>
+    <t>f_v = "top" "end", "top" "head"</t>
+  </si>
+  <si>
+    <t>f_v = "front" "next", "back" "next"</t>
+  </si>
+  <si>
+    <t>f_v = "top" "next"</t>
+  </si>
+  <si>
+    <t>TranslateToImplementation(d_a, f_v) returns implementation of abstraction state</t>
+  </si>
+  <si>
+    <t>d_a = "front"
+f_v = "front" "end", "front" "head", "back" "end", "back" "head"</t>
+  </si>
+  <si>
+    <t>d_a = "ZeroOrMoreData"
+f_v = "front" "end", "front" "head", "back" "end", "back" "head"</t>
+  </si>
+  <si>
+    <t>d_a = "back"
+f_v = "front" "end", "front" "head", "back" "end", "back" "head"</t>
+  </si>
+  <si>
+    <t>d_a = NULL
+f_v = "front" "end", "front" "head", "back" "end", "back" "head"</t>
+  </si>
+  <si>
+    <t>d_i = NULL</t>
+  </si>
+  <si>
+    <t>d_i = "head" "ZeroOrMoreData" "end" NULL,
+"end" "ZeroOrMoreData" "head" NULL</t>
+  </si>
+  <si>
+    <t>SymbolicEvaluation(m_i, D_i)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m_i = Reverse()
+D_i = </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,16 +223,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -84,12 +260,180 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,43 +748,229 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64CF98E1-5D43-4AC7-8948-89C310226CC3}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="32.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.5703125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="38.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="47.140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.28515625" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
+      <c r="I1" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="8"/>
+    </row>
+    <row r="3" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="11"/>
+    </row>
+    <row r="4" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="165" x14ac:dyDescent="0.25">
+      <c r="C8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="255" x14ac:dyDescent="0.25">
+      <c r="E9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="C11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="E12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="E13" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="E14" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="C15" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="E16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="E17" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="E18" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C19" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>